<commit_message>
just for you sira dw
</commit_message>
<xml_diff>
--- a/Track_Model/Track Data.xlsx
+++ b/Track_Model/Track Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d3badd5cb47ce8d/Documents/1140 Project/TRAINS-TEAM2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/aab273_pitt_edu/Documents/Desktop/Trains GIT Location/TRAINS-TEAM2/Track_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{686BC949-9A50-4A63-BA03-574FE949619A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{686BC949-9A50-4A63-BA03-574FE949619A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B94BB89-6FBD-4275-A388-901B390B770C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -5474,8 +5474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -10754,8 +10754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>